<commit_message>
Updates for extra part cooling Fan and bed centring screws
I have updated the printer and assembly manuals. I have issues with part cooling when printing in higher speeds so there is now installed second auxiliary fan on right side and new part fan blowers.
Also new design for bed centring screws now the rotary bed can be adjustable from bottom with screws.
</commit_message>
<xml_diff>
--- a/Assembly Manuals/DUET_6HC_wiring.xlsx
+++ b/Assembly Manuals/DUET_6HC_wiring.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="61">
   <si>
     <t>POWER IN</t>
   </si>
@@ -144,9 +144,6 @@
     <t>24V Led lights</t>
   </si>
   <si>
-    <t>24V Blower radial fan for part cooling</t>
-  </si>
-  <si>
     <t>24V electronics cooling fan (side skirts)</t>
   </si>
   <si>
@@ -190,6 +187,18 @@
   </si>
   <si>
     <t>three wires  (3.3v)+(io4.in)signal (GND)-</t>
+  </si>
+  <si>
+    <t>OUT  6</t>
+  </si>
+  <si>
+    <t>two wires (V_OUTLC1)+ (out6)-</t>
+  </si>
+  <si>
+    <t>24V LEFT SIDE Blower radial fan for part cooling</t>
+  </si>
+  <si>
+    <t>24V RIGHT SIDE Blower radial fan for part cooling</t>
   </si>
 </sst>
 </file>
@@ -273,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -286,6 +295,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -301,13 +313,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>76</xdr:row>
+      <xdr:row>77</xdr:row>
       <xdr:rowOff>61333</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -623,10 +635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N45" sqref="N45"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -641,7 +653,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>16</v>
@@ -652,7 +664,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>16</v>
@@ -663,7 +675,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>17</v>
@@ -777,7 +789,7 @@
         <v>24</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>26</v>
@@ -799,7 +811,7 @@
         <v>29</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>30</v>
@@ -810,7 +822,7 @@
         <v>31</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>32</v>
@@ -842,74 +854,80 @@
         <v>36</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="30" customHeight="1">
       <c r="A23" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+        <v>49</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="30" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>46</v>
+        <v>58</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>48</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>47</v>
       </c>
       <c r="C26" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="2"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="8"/>
-    </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="2"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="8"/>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="9"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="11"/>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="9"/>
@@ -920,6 +938,11 @@
       <c r="A31" s="9"/>
       <c r="B31" s="10"/>
       <c r="C31" s="11"/>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="9"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>